<commit_message>
update significant digits in output tables
</commit_message>
<xml_diff>
--- a/allTrait_Model_univariateANOVA.xlsx
+++ b/allTrait_Model_univariateANOVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apb/Documents/GitHub/microbiome_lifehistory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{415A7A7E-5585-3848-ACDA-1A7F7F178ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0353B694-BCC2-C74F-A56D-66344898A85A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14780" yWindow="7200" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
@@ -972,16 +972,16 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>1.2510667741935599E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>4.3470462817947499</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="F2">
-        <v>3.96997017480889E-2</v>
+        <v>3.9699999999999999E-2</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -995,16 +995,16 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>1.2029697979799E-3</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.417992508097</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="F3">
-        <v>0.51946728607648796</v>
+        <v>0.51900000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1015,16 +1015,16 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>6.8183066767677505E-2</v>
+        <v>6.8199999999999997E-2</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>23.691377070168802</v>
+        <v>23.7</v>
       </c>
       <c r="F4" s="1">
-        <v>4.3820847440743802E-6</v>
+        <v>4.3800000000000004E-6</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -1038,16 +1038,16 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>2.2530906593407601E-3</v>
+        <v>2.2499999999999998E-3</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.78287502915638696</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="F5">
-        <v>0.37845130901033103</v>
+        <v>0.378</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1058,16 +1058,16 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>0.160195398351649</v>
+        <v>0.16</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>55.662641285797797</v>
+        <v>55.7</v>
       </c>
       <c r="F6" s="1">
-        <v>3.6861104519373498E-11</v>
+        <v>3.6900000000000003E-11</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
@@ -1081,16 +1081,16 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>4.12533862433868E-2</v>
+        <v>4.1300000000000003E-2</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>14.3341972610817</v>
+        <v>14.3</v>
       </c>
       <c r="F7" s="1">
-        <v>2.6524632911995299E-4</v>
+        <v>2.6499999999999999E-4</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
@@ -1104,16 +1104,16 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <v>3.8926285714286899E-3</v>
+        <v>3.8899999999999998E-3</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1.3525606232125</v>
+        <v>1.35</v>
       </c>
       <c r="F8">
-        <v>0.24768407599483799</v>
+        <v>0.248</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1124,16 +1124,16 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1.24301075268814</v>
+        <v>1.24</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>5.1970708194288902</v>
+        <v>5.2</v>
       </c>
       <c r="F9">
-        <v>2.4815537592372299E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -1147,16 +1147,16 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>9.8327272727273591</v>
+        <v>9.83</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>41.110971786834298</v>
+        <v>41.1</v>
       </c>
       <c r="F10" s="1">
-        <v>5.2254690174378601E-9</v>
+        <v>5.2300000000000003E-9</v>
       </c>
       <c r="G10" t="s">
         <v>12</v>
@@ -1170,16 +1170,16 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>12.2327272727274</v>
+        <v>12.2</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>51.145454545455202</v>
+        <v>51.1</v>
       </c>
       <c r="F11" s="1">
-        <v>1.6235232182735099E-10</v>
+        <v>1.6200000000000001E-10</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -1193,16 +1193,16 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>9.5253357753358596</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>39.825757336533599</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="F12" s="1">
-        <v>8.3103128448849195E-9</v>
+        <v>8.3099999999999996E-9</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -1216,16 +1216,16 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>11.6586691086691</v>
+        <v>11.7</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>48.7452975664185</v>
+        <v>48.7</v>
       </c>
       <c r="F13" s="1">
-        <v>3.6393348335378202E-10</v>
+        <v>3.6399999999999998E-10</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>
@@ -1239,16 +1239,16 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>0.135449735449725</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0.56632001459583603</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="F14">
-        <v>0.45354735801806501</v>
+        <v>0.45400000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1259,16 +1259,16 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>0.63492063492065398</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>2.65462506841825</v>
+        <v>2.65</v>
       </c>
       <c r="F15">
-        <v>0.106492545889245</v>
+        <v>0.106</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1279,16 +1279,16 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>8.3061346082273607E-6</v>
+        <v>8.3100000000000001E-6</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>0.690539778448782</v>
+        <v>0.69099999999999995</v>
       </c>
       <c r="F16">
-        <v>0.40802165660848999</v>
+        <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1299,16 +1299,16 @@
         <v>10</v>
       </c>
       <c r="C17" s="1">
-        <v>2.7477672900319701E-4</v>
+        <v>2.7500000000000002E-4</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>22.843870286041799</v>
+        <v>22.8</v>
       </c>
       <c r="F17" s="1">
-        <v>6.2507432465505398E-6</v>
+        <v>6.2500000000000003E-6</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -1322,16 +1322,16 @@
         <v>11</v>
       </c>
       <c r="C18" s="1">
-        <v>7.3442875161781299E-4</v>
+        <v>7.3399999999999995E-4</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>61.057554608642803</v>
+        <v>61.1</v>
       </c>
       <c r="F18" s="1">
-        <v>6.6549830736860997E-12</v>
+        <v>6.6500000000000001E-12</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
@@ -1345,16 +1345,16 @@
         <v>13</v>
       </c>
       <c r="C19" s="1">
-        <v>2.7727690801682202E-4</v>
+        <v>2.7700000000000001E-4</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>23.051725460991801</v>
+        <v>23.1</v>
       </c>
       <c r="F19" s="1">
-        <v>5.72771811577039E-6</v>
+        <v>5.7300000000000002E-6</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -1368,16 +1368,16 @@
         <v>14</v>
       </c>
       <c r="C20">
-        <v>1.04116614338454E-3</v>
+        <v>1.0399999999999999E-3</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>86.558510292981296</v>
+        <v>86.6</v>
       </c>
       <c r="F20" s="1">
-        <v>4.2780417237436697E-15</v>
+        <v>4.2800000000000001E-15</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -1391,16 +1391,16 @@
         <v>15</v>
       </c>
       <c r="C21" s="1">
-        <v>3.7176782214891402E-5</v>
+        <v>3.7200000000000003E-5</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>3.0907333151910601</v>
+        <v>3.09</v>
       </c>
       <c r="F21">
-        <v>8.1893685607976496E-2</v>
+        <v>8.1900000000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1411,16 +1411,16 @@
         <v>16</v>
       </c>
       <c r="C22" s="1">
-        <v>1.0278767773017601E-4</v>
+        <v>1.03E-4</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>8.5453683999720909</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="F22">
-        <v>4.3111221247800003E-3</v>
+        <v>4.3099999999999996E-3</v>
       </c>
       <c r="G22" t="s">
         <v>19</v>
@@ -1434,16 +1434,16 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>1.1010752688172001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>1.7499339335106801</v>
+        <v>1.75</v>
       </c>
       <c r="F23">
-        <v>0.18899520364392799</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1454,16 +1454,16 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>6.9337373737373698</v>
+        <v>6.93</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>11.019757377157701</v>
+        <v>11</v>
       </c>
       <c r="F24">
-        <v>1.27089457355868E-3</v>
+        <v>1.2700000000000001E-3</v>
       </c>
       <c r="G24" t="s">
         <v>19</v>
@@ -1477,16 +1477,16 @@
         <v>11</v>
       </c>
       <c r="C25">
-        <v>4.9494949494928104E-3</v>
+        <v>4.9500000000000004E-3</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>7.8662098869601797E-3</v>
+        <v>7.8700000000000003E-3</v>
       </c>
       <c r="F25">
-        <v>0.92950982248365899</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1497,16 +1497,16 @@
         <v>13</v>
       </c>
       <c r="C26" s="1">
-        <v>2.4420024419669002E-4</v>
+        <v>2.4399999999999999E-4</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>3.8810634113182303E-4</v>
+        <v>3.88E-4</v>
       </c>
       <c r="F26">
-        <v>0.98432282688651096</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1517,16 +1517,16 @@
         <v>14</v>
       </c>
       <c r="C27">
-        <v>7.6938339438339298</v>
+        <v>7.69</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>12.227775410462399</v>
+        <v>12.2</v>
       </c>
       <c r="F27" s="1">
-        <v>7.1200430105749504E-4</v>
+        <v>7.1199999999999996E-4</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
@@ -1540,16 +1540,16 @@
         <v>15</v>
       </c>
       <c r="C28" s="1">
-        <v>5.2910052909993499E-4</v>
+        <v>5.2899999999999996E-4</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" s="1">
-        <v>8.4089707246357698E-4</v>
+        <v>8.4099999999999995E-4</v>
       </c>
       <c r="F28">
-        <v>0.97692558518007699</v>
+        <v>0.97699999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1560,16 +1560,16 @@
         <v>16</v>
       </c>
       <c r="C29">
-        <v>1.52539682539682</v>
+        <v>1.53</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>2.4243062599152099</v>
+        <v>2.42</v>
       </c>
       <c r="F29">
-        <v>0.122722946341306</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1580,16 +1580,16 @@
         <v>8</v>
       </c>
       <c r="C30">
-        <v>69.919354838708301</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>0.37643907970516399</v>
+        <v>0.376</v>
       </c>
       <c r="F30">
-        <v>0.540951285488531</v>
+        <v>0.54100000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1600,16 +1600,16 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <v>23275.999999999902</v>
+        <v>23300</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>125.31574468085</v>
+        <v>125</v>
       </c>
       <c r="F31" s="1">
-        <v>3.6220755984726401E-19</v>
+        <v>3.6199999999999998E-19</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
@@ -1623,16 +1623,16 @@
         <v>11</v>
       </c>
       <c r="C32">
-        <v>927.36363636363899</v>
+        <v>927</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>4.9928365991085801</v>
+        <v>4.99</v>
       </c>
       <c r="F32">
-        <v>2.7747948996780999E-2</v>
+        <v>2.7699999999999999E-2</v>
       </c>
       <c r="G32" t="s">
         <v>9</v>
@@ -1646,16 +1646,16 @@
         <v>13</v>
       </c>
       <c r="C33">
-        <v>29.065934065933099</v>
+        <v>29.1</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33">
-        <v>0.1564881926584</v>
+        <v>0.156</v>
       </c>
       <c r="F33">
-        <v>0.69327924493481097</v>
+        <v>0.69299999999999995</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1666,16 +1666,16 @@
         <v>14</v>
       </c>
       <c r="C34">
-        <v>1931.6620879120801</v>
+        <v>1930</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>10.3998828414878</v>
+        <v>10.4</v>
       </c>
       <c r="F34">
-        <v>1.71790409480293E-3</v>
+        <v>1.72E-3</v>
       </c>
       <c r="G34" t="s">
         <v>19</v>
@@ -1689,16 +1689,16 @@
         <v>15</v>
       </c>
       <c r="C35">
-        <v>30.476190476190801</v>
+        <v>30.5</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>0.16408087749438499</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="F35">
-        <v>0.68631876470270603</v>
+        <v>0.68600000000000005</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1709,16 +1709,16 @@
         <v>16</v>
       </c>
       <c r="C36">
-        <v>1372.8571428571399</v>
+        <v>1370</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>7.3913307783797899</v>
+        <v>7.39</v>
       </c>
       <c r="F36">
-        <v>7.7651161011749702E-3</v>
+        <v>7.77E-3</v>
       </c>
       <c r="G36" t="s">
         <v>19</v>
@@ -1732,16 +1732,16 @@
         <v>8</v>
       </c>
       <c r="C37">
-        <v>12.7752688172042</v>
+        <v>12.8</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>1.00901184068136</v>
+        <v>1.01</v>
       </c>
       <c r="F37">
-        <v>0.31763893284460598</v>
+        <v>0.318</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1752,16 +1752,16 @@
         <v>10</v>
       </c>
       <c r="C38">
-        <v>117.818181818181</v>
+        <v>118</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38">
-        <v>9.3054746794839698</v>
+        <v>9.31</v>
       </c>
       <c r="F38">
-        <v>2.9462993227965099E-3</v>
+        <v>2.9499999999999999E-3</v>
       </c>
       <c r="G38" t="s">
         <v>19</v>
@@ -1775,16 +1775,16 @@
         <v>11</v>
       </c>
       <c r="C39">
-        <v>5.8181818181765203E-2</v>
+        <v>5.8200000000000002E-2</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39">
-        <v>4.5952961380126001E-3</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="F39">
-        <v>0.94609344493805703</v>
+        <v>0.94599999999999995</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1795,16 +1795,16 @@
         <v>13</v>
       </c>
       <c r="C40">
-        <v>25.162637362637199</v>
+        <v>25.2</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40">
-        <v>1.9873866769426201</v>
+        <v>1.99</v>
       </c>
       <c r="F40">
-        <v>0.16181266882555201</v>
+        <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1815,16 +1815,16 @@
         <v>14</v>
       </c>
       <c r="C41">
-        <v>2.4664835164835401</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41">
-        <v>0.194806943680574</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="F41">
-        <v>0.65992788799506996</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1835,16 +1835,16 @@
         <v>15</v>
       </c>
       <c r="C42">
-        <v>115.885714285714</v>
+        <v>116</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42">
-        <v>9.1528452006141201</v>
+        <v>9.15</v>
       </c>
       <c r="F42">
-        <v>3.1790204305834802E-3</v>
+        <v>3.1800000000000001E-3</v>
       </c>
       <c r="G42" t="s">
         <v>19</v>
@@ -1858,16 +1858,16 @@
         <v>16</v>
       </c>
       <c r="C43">
-        <v>6.9142857142855902</v>
+        <v>6.91</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43">
-        <v>0.54610171068752</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="F43">
-        <v>0.46169939221551698</v>
+        <v>0.46200000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>